<commit_message>
some AGS fixes. Investigating merge.
</commit_message>
<xml_diff>
--- a/data/municipal_elections/raw_data/thueringen/thueringen_1994.xlsx
+++ b/data/municipal_elections/raw_data/thueringen/thueringen_1994.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10714"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/flosic/Library/CloudStorage/Dropbox/RA_work/Data collection/Germany_Kommunalwahlen/raw_data/thueringen/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/flosic/Documents/GitHub/german_election_data/data/municipal_elections/raw_data/thueringen/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B9DFC23-386E-574F-8ED0-026624FD3423}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65F0F75B-C320-DD45-8F48-46823028BA7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="600" windowWidth="14280" windowHeight="14300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="600" windowWidth="14280" windowHeight="13360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="thueringen_1994" sheetId="2" r:id="rId1"/>
@@ -4646,8 +4646,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:W1248"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A1226" workbookViewId="0">
-      <selection activeCell="E1245" sqref="E1245"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A758" workbookViewId="0">
+      <selection activeCell="B771" sqref="B771"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>